<commit_message>
2022-04-26 오전 09시 34분
</commit_message>
<xml_diff>
--- a/project/기능정의서/JJ_기능정의서0.5.xlsx
+++ b/project/기능정의서/JJ_기능정의서0.5.xlsx
@@ -627,11 +627,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.채용공고 내용호출
- - 클릭시 상세페이지로 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.채용일정을 캘린더형태로 표시
  - 클릭시 상세페이지로 이동</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1333,10 +1328,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>일자리지원센터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1529,6 +1520,15 @@
   </si>
   <si>
     <t>JJ-leader-commute-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.채용공고 목록표시
+ - 클릭시 상세페이지로 이동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2612,9 +2612,9 @@
   </sheetPr>
   <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2698,7 +2698,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2722,7 +2722,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2744,7 +2744,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2768,7 +2768,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2782,7 +2782,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>27</v>
@@ -2792,7 +2792,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2816,7 +2816,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -2840,7 +2840,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -2888,7 +2888,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2912,7 +2912,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2936,7 +2936,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2960,7 +2960,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2984,7 +2984,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3008,7 +3008,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -3016,7 +3016,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>54</v>
@@ -3032,7 +3032,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.3">
@@ -3040,7 +3040,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>54</v>
@@ -3056,7 +3056,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -3078,7 +3078,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3102,7 +3102,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3116,7 +3116,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -3124,7 +3124,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3138,7 +3138,7 @@
         <v>82</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -3146,7 +3146,7 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3160,7 +3160,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -3168,7 +3168,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3176,23 +3176,23 @@
         <v>22</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3200,23 +3200,23 @@
         <v>23</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C25" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="E25" s="33" t="s">
         <v>258</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>259</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3224,23 +3224,23 @@
         <v>24</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="D26" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="D26" s="33" t="s">
-        <v>255</v>
-      </c>
       <c r="E26" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="42"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="81" x14ac:dyDescent="0.3">
@@ -3248,23 +3248,23 @@
         <v>25</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C27" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>255</v>
-      </c>
       <c r="E27" s="33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
       <c r="I27" s="42"/>
       <c r="J27" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="121.5" x14ac:dyDescent="0.3">
@@ -3272,23 +3272,23 @@
         <v>26</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C28" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="D28" s="33" t="s">
         <v>277</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="E28" s="33" t="s">
         <v>278</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>279</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="121.5" x14ac:dyDescent="0.3">
@@ -3296,23 +3296,23 @@
         <v>27</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C29" s="31" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="E29" s="33" t="s">
         <v>282</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>284</v>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3320,23 +3320,23 @@
         <v>28</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D30" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="E30" s="33" t="s">
         <v>264</v>
-      </c>
-      <c r="E30" s="33" t="s">
-        <v>265</v>
       </c>
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3344,23 +3344,23 @@
         <v>29</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C31" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" s="33" t="s">
         <v>266</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>267</v>
       </c>
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
       <c r="I31" s="42"/>
       <c r="J31" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3368,23 +3368,23 @@
         <v>30</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D32" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="E32" s="33" t="s">
         <v>270</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>271</v>
       </c>
       <c r="F32" s="42"/>
       <c r="G32" s="42"/>
       <c r="H32" s="42"/>
       <c r="I32" s="42"/>
       <c r="J32" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3392,23 +3392,23 @@
         <v>31</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C33" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="E33" s="33" t="s">
         <v>286</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>288</v>
       </c>
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="27" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3416,23 +3416,23 @@
         <v>32</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C34" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="E34" s="33" t="s">
         <v>291</v>
-      </c>
-      <c r="D34" s="33" t="s">
-        <v>292</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>293</v>
       </c>
       <c r="F34" s="42"/>
       <c r="G34" s="42"/>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="27" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3440,7 +3440,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C35" s="32" t="s">
         <v>33</v>
@@ -3454,7 +3454,7 @@
         <v>85</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3489,14 +3489,14 @@
         <v>90</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F37" s="26"/>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
       <c r="J37" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -3510,7 +3510,7 @@
         <v>89</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E38" s="34" t="s">
         <v>120</v>
@@ -3520,7 +3520,7 @@
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="202.5" x14ac:dyDescent="0.3">
@@ -3528,13 +3528,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C39" s="31" t="s">
         <v>89</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E39" s="34"/>
       <c r="F39" s="5"/>
@@ -3542,7 +3542,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -3550,13 +3550,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C40" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="D40" s="26" t="s">
         <v>237</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>238</v>
       </c>
       <c r="E40" s="34"/>
       <c r="F40" s="5"/>
@@ -3564,7 +3564,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -3572,13 +3572,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C41" s="31" t="s">
         <v>89</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E41" s="34"/>
       <c r="F41" s="5"/>
@@ -3586,7 +3586,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="27" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -3600,17 +3600,17 @@
         <v>89</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="34" t="s">
         <v>209</v>
-      </c>
-      <c r="E42" s="34" t="s">
-        <v>210</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="121.5" x14ac:dyDescent="0.3">
@@ -3627,14 +3627,14 @@
         <v>107</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -3651,14 +3651,14 @@
         <v>107</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="297" x14ac:dyDescent="0.3">
@@ -3675,14 +3675,14 @@
         <v>107</v>
       </c>
       <c r="E45" s="34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
@@ -3699,14 +3699,14 @@
         <v>107</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="81" x14ac:dyDescent="0.3">
@@ -3723,14 +3723,14 @@
         <v>107</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="171.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3747,7 +3747,7 @@
         <v>107</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -3769,14 +3769,14 @@
         <v>107</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="67.5" x14ac:dyDescent="0.3">
@@ -3793,14 +3793,14 @@
         <v>109</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="121.5" x14ac:dyDescent="0.3">
@@ -3814,17 +3814,17 @@
         <v>89</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E51" s="34" t="s">
         <v>224</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>225</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3841,14 +3841,14 @@
         <v>109</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="121.5" x14ac:dyDescent="0.3">
@@ -3865,14 +3865,14 @@
         <v>109</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.3">
@@ -3889,14 +3889,14 @@
         <v>109</v>
       </c>
       <c r="E54" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3920,7 +3920,7 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -3944,7 +3944,7 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -3968,7 +3968,7 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3976,7 +3976,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C58" s="32" t="s">
         <v>115</v>
@@ -3998,7 +3998,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C59" s="32" t="s">
         <v>84</v>
@@ -4012,7 +4012,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4020,7 +4020,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C60" s="32" t="s">
         <v>123</v>
@@ -4042,7 +4042,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C61" s="32" t="s">
         <v>123</v>
@@ -4066,7 +4066,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C62" s="32" t="s">
         <v>123</v>
@@ -4080,7 +4080,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4088,7 +4088,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C63" s="32" t="s">
         <v>84</v>
@@ -4112,7 +4112,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C64" s="32" t="s">
         <v>84</v>
@@ -4134,7 +4134,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C65" s="32" t="s">
         <v>129</v>
@@ -4154,7 +4154,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C66" s="32" t="s">
         <v>129</v>
@@ -4168,7 +4168,7 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="35" t="s">
-        <v>153</v>
+        <v>333</v>
       </c>
       <c r="L66" s="43"/>
     </row>
@@ -4177,7 +4177,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C67" s="32" t="s">
         <v>135</v>
@@ -4191,7 +4191,7 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L67" s="43"/>
     </row>
@@ -4200,7 +4200,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C68" s="32" t="s">
         <v>129</v>
@@ -4214,7 +4214,7 @@
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L68" s="43"/>
     </row>
@@ -4245,7 +4245,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C70" s="32" t="s">
         <v>137</v>
@@ -4261,7 +4261,7 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="27" x14ac:dyDescent="0.3">
@@ -4269,7 +4269,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C71" s="32" t="s">
         <v>140</v>
@@ -4285,7 +4285,7 @@
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4293,7 +4293,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C72" s="32" t="s">
         <v>143</v>
@@ -4309,7 +4309,7 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -4317,23 +4317,23 @@
         <v>71</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C73" s="32" t="s">
         <v>137</v>
       </c>
       <c r="D73" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="67.5" x14ac:dyDescent="0.3">
@@ -4341,23 +4341,23 @@
         <v>72</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C74" s="32" t="s">
         <v>137</v>
       </c>
       <c r="D74" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -4365,23 +4365,23 @@
         <v>73</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D75" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="94.5" x14ac:dyDescent="0.3">
@@ -4389,23 +4389,23 @@
         <v>74</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C76" s="32" t="s">
         <v>83</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="77" spans="1:12" ht="162" x14ac:dyDescent="0.3">
@@ -4413,23 +4413,23 @@
         <v>75</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C77" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="D77" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="D77" s="32" t="s">
+      <c r="E77" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:12" ht="54" x14ac:dyDescent="0.3">
@@ -4437,13 +4437,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C78" s="32" t="s">
         <v>137</v>
       </c>
       <c r="D78" s="32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>146</v>
@@ -4453,7 +4453,7 @@
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="27" x14ac:dyDescent="0.3">
@@ -4461,23 +4461,23 @@
         <v>77</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C79" s="32" t="s">
         <v>147</v>
       </c>
       <c r="D79" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="67.5" x14ac:dyDescent="0.3">
@@ -4485,13 +4485,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D80" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -4499,7 +4499,7 @@
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="40.5" x14ac:dyDescent="0.3">
@@ -4513,17 +4513,17 @@
         <v>113</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -4531,23 +4531,23 @@
         <v>80</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C82" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="D82" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="D82" s="32" t="s">
+      <c r="E82" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>